<commit_message>
Commit 082322 Change Profil pic dan Change Email
</commit_message>
<xml_diff>
--- a/Profile - Change Email/Default.xlsx
+++ b/Profile - Change Email/Default.xlsx
@@ -14,6 +14,41 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+  <si>
+    <t>PROJECT_NAME</t>
+  </si>
+  <si>
+    <t>SuperApps-BSI Super Apps versi 1.0.2 (7761)</t>
+  </si>
+  <si>
+    <t>COMPANY_LOGO</t>
+  </si>
+  <si>
+    <t>SCREEN_SHOOT</t>
+  </si>
+  <si>
+    <t>COVER_TITLE</t>
+  </si>
+  <si>
+    <t>D:\Mentahan\PlugIn UFT\Napalm\Napalm\libray\BSILOGO.jpeg</t>
+  </si>
+  <si>
+    <t>SuperApps-BSIMobile</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>COVER_SUBTITLE</t>
+  </si>
+  <si>
+    <t>Automation Testing - SuperApps-BSIMobile</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
@@ -154,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,13 +197,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -467,16 +532,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.75390625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.48828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.37109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.3671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" customFormat="1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -492,10 +600,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="15.1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
menyelesaikan change pic 100%
</commit_message>
<xml_diff>
--- a/Profile - Change Email/Default.xlsx
+++ b/Profile - Change Email/Default.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="Change Email - Positive" sheetId="2" r:id="rId2"/>
+    <sheet name="Change Email - Negative" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -535,7 +536,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -549,7 +550,7 @@
     <col min="7" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1">
+    <row r="1" ht="14.95" customFormat="1">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -594,7 +595,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +604,26 @@
     <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1"/>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Menyelesaikan Error pada function library bsi mobile - profile
</commit_message>
<xml_diff>
--- a/Profile - Change Email/Default.xlsx
+++ b/Profile - Change Email/Default.xlsx
@@ -249,10 +249,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="283845"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -536,16 +536,16 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="1" width="10.75390625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.48828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.37109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.86328125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52.3671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.53515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
@@ -623,7 +623,7 @@
     <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>